<commit_message>
Make BELLHOP ver a parameter; update settings file
</commit_message>
<xml_diff>
--- a/PropaMod_Settings_ConfigV2.xlsx
+++ b/PropaMod_Settings_ConfigV2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>Bathymetry Model</t>
   </si>
@@ -1255,6 +1255,57 @@
   </si>
   <si>
     <t>ElevFromBot</t>
+  </si>
+  <si>
+    <t>BELLHOP Version</t>
+  </si>
+  <si>
+    <t>jah</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jah</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Use BELLHOP version bellhop_jah.exe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cxx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Use BELLhop version bellhopcxx.exe</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1265,7 +1316,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1334,22 +1385,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFA709F5"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1449,10 +1489,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1739,10 +1783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,7 +1890,7 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="20" t="s">
         <v>105</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1857,7 +1901,7 @@
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="20" t="s">
         <v>104</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1868,7 +1912,7 @@
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="20" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1876,7 +1920,7 @@
       <c r="A14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="20" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1887,44 +1931,44 @@
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="10">
         <v>32.25</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="10">
         <v>-119</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="10" t="s">
         <v>112</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="21">
         <v>1000</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -1935,7 +1979,7 @@
       <c r="A21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="10">
         <v>220</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1979,312 +2023,323 @@
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+    <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+    <row r="34" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C34" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13" t="s">
+      <c r="B35" s="13"/>
+      <c r="C35" s="13" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="14">
-        <v>1550</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="15">
-        <v>129.9</v>
+        <v>21</v>
+      </c>
+      <c r="B36" s="14">
+        <v>1550</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="16">
-        <v>1.1399999999999999</v>
+        <v>22</v>
+      </c>
+      <c r="B37" s="15">
+        <v>129.9</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="2">
-        <v>1.5E-3</v>
+        <v>19</v>
+      </c>
+      <c r="B38" s="16">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="17">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B41" s="15">
         <v>30</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13" t="s">
+      <c r="B42" s="13"/>
+      <c r="C42" s="13" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B44" s="2">
         <v>1</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C44" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="15">
-        <v>10000</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47" s="15">
-        <v>10</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>61</v>
+        <v>10000</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" s="15">
         <v>10</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="15">
+        <v>10</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B50" s="15">
         <v>16</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C50" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="B52" s="2">
-        <v>0</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="B53" s="2">
         <v>0</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>94</v>
+      <c r="C53" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B54" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="2">
+        <v>100</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B56" s="2">
         <v>200</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C56" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
+    <row r="57" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="18" t="s">
+      <c r="B57" s="12"/>
+      <c r="C57" s="18" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B57" s="2">
-        <v>0</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B58" s="2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B59" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B60" s="2">
         <v>10</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Multiple frequencies and directories from the save date
Re-install functionality to deal with multiple frequencies and generate more than one directory for each day when needed
</commit_message>
<xml_diff>
--- a/PropaMod_Settings_ConfigV2.xlsx
+++ b/PropaMod_Settings_ConfigV2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\PropaMod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nposd\Documents\GitHub\PropaMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -152,9 +152,6 @@
     <t>[dB]</t>
   </si>
   <si>
-    <t>[Hz]</t>
-  </si>
-  <si>
     <t>Value (EDIT)</t>
   </si>
   <si>
@@ -1306,6 +1303,10 @@
       </rPr>
       <t xml:space="preserve"> - Use BELLhop version bellhopcxx.exe</t>
     </r>
+  </si>
+  <si>
+    <t>[Hz] 
+Enter multiple frequencies as [1000 2000] or [1000 2000 3000]</t>
   </si>
 </sst>
 </file>
@@ -1785,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,15 +1803,15 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1822,7 +1823,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1830,12 +1831,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1845,7 +1846,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1853,7 +1854,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1861,10 +1862,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1872,10 +1873,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1883,7 +1884,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1891,10 +1892,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1902,10 +1903,10 @@
         <v>38</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1913,20 +1914,20 @@
         <v>10</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1955,24 +1956,24 @@
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="21">
         <v>1000</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1986,20 +1987,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="2">
         <v>40000</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>42</v>
+      <c r="C22" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2012,25 +2013,25 @@
         <v>18</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2041,51 +2042,51 @@
         <v>17</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -2093,19 +2094,19 @@
         <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2116,7 +2117,7 @@
         <v>1550</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2127,7 +2128,7 @@
         <v>129.9</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2138,7 +2139,7 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2165,27 +2166,27 @@
         <v>30</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -2196,12 +2197,12 @@
         <v>1</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -2214,7 +2215,7 @@
         <v>10000</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2225,7 +2226,7 @@
         <v>10</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2236,7 +2237,7 @@
         <v>10</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2247,12 +2248,12 @@
         <v>16</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -2265,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2276,7 +2277,7 @@
         <v>0</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2287,7 +2288,7 @@
         <v>100</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2298,16 +2299,16 @@
         <v>200</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2318,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,7 +2330,7 @@
         <v>2000</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2340,7 +2341,7 @@
         <v>10</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>